<commit_message>
+ Added NaiveBayes model + Added scripts to analyse per group based on PCA and Naive Bayes
</commit_message>
<xml_diff>
--- a/Data/out/Re-organization_0.xlsx
+++ b/Data/out/Re-organization_0.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="751" uniqueCount="605">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1145" uniqueCount="927">
   <si>
     <t>Label</t>
   </si>
@@ -859,6 +859,972 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>IInj</t>
+  </si>
+  <si>
+    <t>ADP</t>
+  </si>
+  <si>
+    <t>LabelPrediction</t>
+  </si>
+  <si>
+    <t>Label</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Experiment</t>
+  </si>
+  <si>
+    <t>CFA d1</t>
+  </si>
+  <si>
+    <t>Slice</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>t1</t>
+  </si>
+  <si>
+    <t>t3</t>
+  </si>
+  <si>
+    <t>t8</t>
+  </si>
+  <si>
+    <t>t12</t>
+  </si>
+  <si>
+    <t>t45</t>
+  </si>
+  <si>
+    <t>t61</t>
+  </si>
+  <si>
+    <t>t8</t>
+  </si>
+  <si>
+    <t>t1</t>
+  </si>
+  <si>
+    <t>t3</t>
+  </si>
+  <si>
+    <t>t1</t>
+  </si>
+  <si>
+    <t>t14</t>
+  </si>
+  <si>
+    <t>t1</t>
+  </si>
+  <si>
+    <t>t26</t>
+  </si>
+  <si>
+    <t>t30</t>
+  </si>
+  <si>
+    <t>t3</t>
+  </si>
+  <si>
+    <t>Depth</t>
+  </si>
+  <si>
+    <t>Bifurcation</t>
+  </si>
+  <si>
+    <t>Polarity</t>
+  </si>
+  <si>
+    <t>Perimeter</t>
+  </si>
+  <si>
+    <t>Area</t>
+  </si>
+  <si>
+    <t>Diameter</t>
+  </si>
+  <si>
+    <t>Measured</t>
+  </si>
+  <si>
+    <t>MaxH</t>
+  </si>
+  <si>
+    <t>MaxV</t>
+  </si>
+  <si>
+    <t>Den</t>
+  </si>
+  <si>
+    <t>MaxH_1</t>
+  </si>
+  <si>
+    <t>MaxV_1</t>
+  </si>
+  <si>
+    <t>Angle</t>
+  </si>
+  <si>
+    <t>MaxOrder</t>
+  </si>
+  <si>
+    <t>Oblique</t>
+  </si>
+  <si>
+    <t>SAG</t>
+  </si>
+  <si>
+    <t>SAGAmp</t>
+  </si>
+  <si>
+    <t>InputR</t>
+  </si>
+  <si>
+    <t>RMP</t>
+  </si>
+  <si>
+    <t>APThreshold</t>
+  </si>
+  <si>
+    <t>Tau</t>
+  </si>
+  <si>
+    <t>Cap</t>
+  </si>
+  <si>
+    <t>Adaptation</t>
+  </si>
+  <si>
+    <t>SpikeCount</t>
+  </si>
+  <si>
+    <t>APAmplitude</t>
+  </si>
+  <si>
+    <t>APHW</t>
+  </si>
+  <si>
+    <t>VeloDepo</t>
+  </si>
+  <si>
+    <t>VelRepo</t>
+  </si>
+  <si>
+    <t>ICAmp</t>
+  </si>
+  <si>
+    <t>Burst</t>
+  </si>
+  <si>
+    <t>IInj</t>
+  </si>
+  <si>
+    <t>ADP</t>
+  </si>
+  <si>
+    <t>LabelPrediction</t>
+  </si>
+  <si>
+    <t>Label</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Experiment</t>
+  </si>
+  <si>
+    <t>CFA d7</t>
+  </si>
+  <si>
+    <t>Slice</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>t10</t>
+  </si>
+  <si>
+    <t>t6</t>
+  </si>
+  <si>
+    <t>t8</t>
+  </si>
+  <si>
+    <t>t3</t>
+  </si>
+  <si>
+    <t>t1</t>
+  </si>
+  <si>
+    <t>t4</t>
+  </si>
+  <si>
+    <t>t5</t>
+  </si>
+  <si>
+    <t>t1</t>
+  </si>
+  <si>
+    <t>t23</t>
+  </si>
+  <si>
+    <t>t1</t>
+  </si>
+  <si>
+    <t>t3</t>
+  </si>
+  <si>
+    <t>t12</t>
+  </si>
+  <si>
+    <t>t4</t>
+  </si>
+  <si>
+    <t>t18</t>
+  </si>
+  <si>
+    <t>t25</t>
+  </si>
+  <si>
+    <t>Depth</t>
+  </si>
+  <si>
+    <t>Bifurcation</t>
+  </si>
+  <si>
+    <t>Polarity</t>
+  </si>
+  <si>
+    <t>Perimeter</t>
+  </si>
+  <si>
+    <t>Area</t>
+  </si>
+  <si>
+    <t>Diameter</t>
+  </si>
+  <si>
+    <t>Measured</t>
+  </si>
+  <si>
+    <t>MaxH</t>
+  </si>
+  <si>
+    <t>MaxV</t>
+  </si>
+  <si>
+    <t>Den</t>
+  </si>
+  <si>
+    <t>MaxH_1</t>
+  </si>
+  <si>
+    <t>MaxV_1</t>
+  </si>
+  <si>
+    <t>Angle</t>
+  </si>
+  <si>
+    <t>MaxOrder</t>
+  </si>
+  <si>
+    <t>Oblique</t>
+  </si>
+  <si>
+    <t>SAG</t>
+  </si>
+  <si>
+    <t>SAGAmp</t>
+  </si>
+  <si>
+    <t>InputR</t>
+  </si>
+  <si>
+    <t>RMP</t>
+  </si>
+  <si>
+    <t>APThreshold</t>
+  </si>
+  <si>
+    <t>Tau</t>
+  </si>
+  <si>
+    <t>Cap</t>
+  </si>
+  <si>
+    <t>Adaptation</t>
+  </si>
+  <si>
+    <t>SpikeCount</t>
+  </si>
+  <si>
+    <t>APAmplitude</t>
+  </si>
+  <si>
+    <t>APHW</t>
+  </si>
+  <si>
+    <t>VeloDepo</t>
+  </si>
+  <si>
+    <t>VelRepo</t>
+  </si>
+  <si>
+    <t>ICAmp</t>
+  </si>
+  <si>
+    <t>Burst</t>
+  </si>
+  <si>
+    <t>IInj</t>
+  </si>
+  <si>
+    <t>ADP</t>
+  </si>
+  <si>
+    <t>LabelPrediction</t>
+  </si>
+  <si>
+    <t>Label</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Experiment</t>
+  </si>
+  <si>
+    <t>CFA d7NS</t>
+  </si>
+  <si>
+    <t>Slice</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>t3</t>
+  </si>
+  <si>
+    <t>t16</t>
+  </si>
+  <si>
+    <t>t12</t>
+  </si>
+  <si>
+    <t>t7</t>
+  </si>
+  <si>
+    <t>Depth</t>
+  </si>
+  <si>
+    <t>Bifurcation</t>
+  </si>
+  <si>
+    <t>Polarity</t>
+  </si>
+  <si>
+    <t>Perimeter</t>
+  </si>
+  <si>
+    <t>Area</t>
+  </si>
+  <si>
+    <t>Diameter</t>
+  </si>
+  <si>
+    <t>Measured</t>
+  </si>
+  <si>
+    <t>MaxH</t>
+  </si>
+  <si>
+    <t>MaxV</t>
+  </si>
+  <si>
+    <t>Den</t>
+  </si>
+  <si>
+    <t>MaxH_1</t>
+  </si>
+  <si>
+    <t>MaxV_1</t>
+  </si>
+  <si>
+    <t>Angle</t>
+  </si>
+  <si>
+    <t>MaxOrder</t>
+  </si>
+  <si>
+    <t>Oblique</t>
+  </si>
+  <si>
+    <t>SAG</t>
+  </si>
+  <si>
+    <t>SAGAmp</t>
+  </si>
+  <si>
+    <t>InputR</t>
+  </si>
+  <si>
+    <t>RMP</t>
+  </si>
+  <si>
+    <t>APThreshold</t>
+  </si>
+  <si>
+    <t>Tau</t>
+  </si>
+  <si>
+    <t>Cap</t>
+  </si>
+  <si>
+    <t>Adaptation</t>
+  </si>
+  <si>
+    <t>SpikeCount</t>
+  </si>
+  <si>
+    <t>APAmplitude</t>
+  </si>
+  <si>
+    <t>APHW</t>
+  </si>
+  <si>
+    <t>VeloDepo</t>
+  </si>
+  <si>
+    <t>VelRepo</t>
+  </si>
+  <si>
+    <t>ICAmp</t>
+  </si>
+  <si>
+    <t>Burst</t>
+  </si>
+  <si>
+    <t>IInj</t>
+  </si>
+  <si>
+    <t>ADP</t>
+  </si>
+  <si>
+    <t>LabelPrediction</t>
+  </si>
+  <si>
+    <t>Label</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Experiment</t>
+  </si>
+  <si>
+    <t>Saline d1</t>
+  </si>
+  <si>
+    <t>Slice</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>t18</t>
+  </si>
+  <si>
+    <t>t8</t>
+  </si>
+  <si>
+    <t>t2</t>
+  </si>
+  <si>
+    <t>t10</t>
+  </si>
+  <si>
+    <t>t9</t>
+  </si>
+  <si>
+    <t>Depth</t>
+  </si>
+  <si>
+    <t>Bifurcation</t>
+  </si>
+  <si>
+    <t>Polarity</t>
+  </si>
+  <si>
+    <t>Perimeter</t>
+  </si>
+  <si>
+    <t>Area</t>
+  </si>
+  <si>
+    <t>Diameter</t>
+  </si>
+  <si>
+    <t>Measured</t>
+  </si>
+  <si>
+    <t>MaxH</t>
+  </si>
+  <si>
+    <t>MaxV</t>
+  </si>
+  <si>
+    <t>Den</t>
+  </si>
+  <si>
+    <t>MaxH_1</t>
+  </si>
+  <si>
+    <t>MaxV_1</t>
+  </si>
+  <si>
+    <t>Angle</t>
+  </si>
+  <si>
+    <t>MaxOrder</t>
+  </si>
+  <si>
+    <t>Oblique</t>
+  </si>
+  <si>
+    <t>SAG</t>
+  </si>
+  <si>
+    <t>SAGAmp</t>
+  </si>
+  <si>
+    <t>InputR</t>
+  </si>
+  <si>
+    <t>RMP</t>
+  </si>
+  <si>
+    <t>APThreshold</t>
+  </si>
+  <si>
+    <t>Tau</t>
+  </si>
+  <si>
+    <t>Cap</t>
+  </si>
+  <si>
+    <t>Adaptation</t>
+  </si>
+  <si>
+    <t>SpikeCount</t>
+  </si>
+  <si>
+    <t>APAmplitude</t>
+  </si>
+  <si>
+    <t>APHW</t>
+  </si>
+  <si>
+    <t>VeloDepo</t>
+  </si>
+  <si>
+    <t>VelRepo</t>
+  </si>
+  <si>
+    <t>ICAmp</t>
+  </si>
+  <si>
+    <t>Burst</t>
+  </si>
+  <si>
+    <t>IInj</t>
+  </si>
+  <si>
+    <t>ADP</t>
+  </si>
+  <si>
+    <t>LabelPrediction</t>
+  </si>
+  <si>
+    <t>Label</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Experiment</t>
+  </si>
+  <si>
+    <t>Saline d7</t>
+  </si>
+  <si>
+    <t>Slice</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>t14</t>
+  </si>
+  <si>
+    <t>t3</t>
+  </si>
+  <si>
+    <t>t14</t>
+  </si>
+  <si>
+    <t>t6</t>
+  </si>
+  <si>
+    <t>Depth</t>
+  </si>
+  <si>
+    <t>Bifurcation</t>
+  </si>
+  <si>
+    <t>Polarity</t>
+  </si>
+  <si>
+    <t>Perimeter</t>
+  </si>
+  <si>
+    <t>Area</t>
+  </si>
+  <si>
+    <t>Diameter</t>
+  </si>
+  <si>
+    <t>Measured</t>
+  </si>
+  <si>
+    <t>MaxH</t>
+  </si>
+  <si>
+    <t>MaxV</t>
+  </si>
+  <si>
+    <t>Den</t>
+  </si>
+  <si>
+    <t>MaxH_1</t>
+  </si>
+  <si>
+    <t>MaxV_1</t>
+  </si>
+  <si>
+    <t>Angle</t>
+  </si>
+  <si>
+    <t>MaxOrder</t>
+  </si>
+  <si>
+    <t>Oblique</t>
+  </si>
+  <si>
+    <t>SAG</t>
+  </si>
+  <si>
+    <t>SAGAmp</t>
+  </si>
+  <si>
+    <t>InputR</t>
+  </si>
+  <si>
+    <t>RMP</t>
+  </si>
+  <si>
+    <t>APThreshold</t>
+  </si>
+  <si>
+    <t>Tau</t>
+  </si>
+  <si>
+    <t>Cap</t>
+  </si>
+  <si>
+    <t>Adaptation</t>
+  </si>
+  <si>
+    <t>SpikeCount</t>
+  </si>
+  <si>
+    <t>APAmplitude</t>
+  </si>
+  <si>
+    <t>APHW</t>
+  </si>
+  <si>
+    <t>VeloDepo</t>
+  </si>
+  <si>
+    <t>VelRepo</t>
+  </si>
+  <si>
+    <t>ICAmp</t>
+  </si>
+  <si>
+    <t>Burst</t>
+  </si>
+  <si>
+    <t>IInj</t>
+  </si>
+  <si>
+    <t>ADP</t>
+  </si>
+  <si>
+    <t>LabelPrediction</t>
+  </si>
+  <si>
+    <t>Label</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Experiment</t>
+  </si>
+  <si>
+    <t>Saline d7NS</t>
+  </si>
+  <si>
+    <t>Slice</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>t23</t>
+  </si>
+  <si>
+    <t>t5</t>
+  </si>
+  <si>
+    <t>t10</t>
+  </si>
+  <si>
+    <t>t8</t>
+  </si>
+  <si>
+    <t>t30</t>
+  </si>
+  <si>
+    <t>t38</t>
+  </si>
+  <si>
+    <t>t20</t>
+  </si>
+  <si>
+    <t>t5</t>
+  </si>
+  <si>
+    <t>t18</t>
+  </si>
+  <si>
+    <t>t3</t>
+  </si>
+  <si>
+    <t>t23</t>
+  </si>
+  <si>
+    <t>t6</t>
+  </si>
+  <si>
+    <t>Depth</t>
+  </si>
+  <si>
+    <t>Bifurcation</t>
+  </si>
+  <si>
+    <t>Polarity</t>
+  </si>
+  <si>
+    <t>Perimeter</t>
+  </si>
+  <si>
+    <t>Area</t>
+  </si>
+  <si>
+    <t>Diameter</t>
+  </si>
+  <si>
+    <t>Measured</t>
+  </si>
+  <si>
+    <t>MaxH</t>
+  </si>
+  <si>
+    <t>MaxV</t>
+  </si>
+  <si>
+    <t>Den</t>
+  </si>
+  <si>
+    <t>MaxH_1</t>
+  </si>
+  <si>
+    <t>MaxV_1</t>
+  </si>
+  <si>
+    <t>Angle</t>
+  </si>
+  <si>
+    <t>MaxOrder</t>
+  </si>
+  <si>
+    <t>Oblique</t>
+  </si>
+  <si>
+    <t>SAG</t>
+  </si>
+  <si>
+    <t>SAGAmp</t>
+  </si>
+  <si>
+    <t>InputR</t>
+  </si>
+  <si>
+    <t>RMP</t>
+  </si>
+  <si>
+    <t>APThreshold</t>
+  </si>
+  <si>
+    <t>Tau</t>
+  </si>
+  <si>
+    <t>Cap</t>
+  </si>
+  <si>
+    <t>Adaptation</t>
+  </si>
+  <si>
+    <t>SpikeCount</t>
+  </si>
+  <si>
+    <t>APAmplitude</t>
+  </si>
+  <si>
+    <t>APHW</t>
+  </si>
+  <si>
+    <t>VeloDepo</t>
+  </si>
+  <si>
+    <t>VelRepo</t>
+  </si>
+  <si>
+    <t>ICAmp</t>
+  </si>
+  <si>
+    <t>Burst</t>
   </si>
   <si>
     <t>IInj</t>
@@ -1904,177 +2870,177 @@
   <dimension ref="A1:AL16"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="5.48828125" customWidth="true"/>
-    <col min="2" max="2" width="7.15625" customWidth="true"/>
-    <col min="3" max="3" width="10.37890625" customWidth="true"/>
-    <col min="4" max="4" width="4.82421875" customWidth="true"/>
-    <col min="5" max="5" width="3.82421875" customWidth="true"/>
+    <col min="1" max="1" width="5.85546875" customWidth="true"/>
+    <col min="2" max="2" width="7.140625" customWidth="true"/>
+    <col min="3" max="3" width="11.42578125" customWidth="true"/>
+    <col min="4" max="4" width="5.28515625" customWidth="true"/>
+    <col min="5" max="5" width="3.85546875" customWidth="true"/>
     <col min="6" max="6" width="7.7109375" customWidth="true"/>
-    <col min="7" max="7" width="10.15625" customWidth="true"/>
-    <col min="8" max="8" width="7.37890625" customWidth="true"/>
-    <col min="9" max="9" width="9.15625" customWidth="true"/>
+    <col min="7" max="7" width="10.85546875" customWidth="true"/>
+    <col min="8" max="8" width="8" customWidth="true"/>
+    <col min="9" max="9" width="10.140625" customWidth="true"/>
     <col min="10" max="10" width="7.7109375" customWidth="true"/>
-    <col min="11" max="11" width="8.7109375" customWidth="true"/>
-    <col min="12" max="12" width="9.26953125" customWidth="true"/>
+    <col min="11" max="11" width="9.42578125" customWidth="true"/>
+    <col min="12" max="12" width="10" customWidth="true"/>
     <col min="13" max="13" width="7.7109375" customWidth="true"/>
     <col min="14" max="14" width="7.7109375" customWidth="true"/>
-    <col min="15" max="15" width="4.37890625" customWidth="true"/>
-    <col min="16" max="16" width="7.93359375" customWidth="true"/>
-    <col min="17" max="17" width="7.82421875" customWidth="true"/>
+    <col min="15" max="15" width="4.7109375" customWidth="true"/>
+    <col min="16" max="16" width="8.140625" customWidth="true"/>
+    <col min="17" max="17" width="8.140625" customWidth="true"/>
     <col min="18" max="18" width="6.7109375" customWidth="true"/>
-    <col min="19" max="19" width="9.37890625" customWidth="true"/>
-    <col min="20" max="20" width="7.37890625" customWidth="true"/>
+    <col min="19" max="19" width="10" customWidth="true"/>
+    <col min="20" max="20" width="8.28515625" customWidth="true"/>
     <col min="21" max="21" width="11.7109375" customWidth="true"/>
-    <col min="22" max="22" width="8.7109375" customWidth="true"/>
+    <col min="22" max="22" width="8.85546875" customWidth="true"/>
     <col min="23" max="23" width="11.7109375" customWidth="true"/>
-    <col min="24" max="24" width="10.37890625" customWidth="true"/>
-    <col min="25" max="25" width="11.7109375" customWidth="true"/>
+    <col min="24" max="24" width="10.42578125" customWidth="true"/>
+    <col min="25" max="25" width="12.42578125" customWidth="true"/>
     <col min="26" max="26" width="11.7109375" customWidth="true"/>
     <col min="27" max="27" width="13.7109375" customWidth="true"/>
     <col min="28" max="28" width="12.7109375" customWidth="true"/>
-    <col min="29" max="29" width="10.26953125" customWidth="true"/>
-    <col min="30" max="30" width="11.48828125" customWidth="true"/>
+    <col min="29" max="29" width="11.28515625" customWidth="true"/>
+    <col min="30" max="30" width="13" customWidth="true"/>
     <col min="31" max="31" width="12.7109375" customWidth="true"/>
-    <col min="32" max="32" width="9.7109375" customWidth="true"/>
+    <col min="32" max="32" width="10" customWidth="true"/>
     <col min="33" max="33" width="8.7109375" customWidth="true"/>
     <col min="34" max="34" width="8.7109375" customWidth="true"/>
     <col min="35" max="35" width="11.7109375" customWidth="true"/>
-    <col min="36" max="36" width="3.7109375" customWidth="true"/>
+    <col min="36" max="36" width="4" customWidth="true"/>
     <col min="37" max="37" width="7.7109375" customWidth="true"/>
-    <col min="38" max="38" width="13.7109375" customWidth="true"/>
+    <col min="38" max="38" width="15" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>283</v>
+        <v>605</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>292</v>
+        <v>614</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>293</v>
+        <v>615</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>295</v>
+        <v>617</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>296</v>
+        <v>618</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>312</v>
+        <v>634</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>313</v>
+        <v>635</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>314</v>
+        <v>636</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>315</v>
+        <v>637</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>316</v>
+        <v>638</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>317</v>
+        <v>639</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>318</v>
+        <v>640</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>319</v>
+        <v>641</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>320</v>
+        <v>642</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>321</v>
+        <v>643</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>322</v>
+        <v>644</v>
       </c>
       <c r="Q1" s="0" t="s">
-        <v>323</v>
+        <v>645</v>
       </c>
       <c r="R1" s="0" t="s">
-        <v>324</v>
+        <v>646</v>
       </c>
       <c r="S1" s="0" t="s">
-        <v>325</v>
+        <v>647</v>
       </c>
       <c r="T1" s="0" t="s">
-        <v>326</v>
+        <v>648</v>
       </c>
       <c r="U1" s="0" t="s">
-        <v>327</v>
+        <v>649</v>
       </c>
       <c r="V1" s="0" t="s">
-        <v>328</v>
+        <v>650</v>
       </c>
       <c r="W1" s="0" t="s">
-        <v>329</v>
+        <v>651</v>
       </c>
       <c r="X1" s="0" t="s">
-        <v>330</v>
+        <v>652</v>
       </c>
       <c r="Y1" s="0" t="s">
-        <v>331</v>
+        <v>653</v>
       </c>
       <c r="Z1" s="0" t="s">
-        <v>332</v>
+        <v>654</v>
       </c>
       <c r="AA1" s="0" t="s">
-        <v>333</v>
+        <v>655</v>
       </c>
       <c r="AB1" s="0" t="s">
-        <v>334</v>
+        <v>656</v>
       </c>
       <c r="AC1" s="0" t="s">
-        <v>335</v>
+        <v>657</v>
       </c>
       <c r="AD1" s="0" t="s">
-        <v>336</v>
+        <v>658</v>
       </c>
       <c r="AE1" s="0" t="s">
-        <v>337</v>
+        <v>659</v>
       </c>
       <c r="AF1" s="0" t="s">
-        <v>338</v>
+        <v>660</v>
       </c>
       <c r="AG1" s="0" t="s">
-        <v>339</v>
+        <v>661</v>
       </c>
       <c r="AH1" s="0" t="s">
-        <v>340</v>
+        <v>662</v>
       </c>
       <c r="AI1" s="0" t="s">
-        <v>341</v>
+        <v>663</v>
       </c>
       <c r="AJ1" s="0" t="s">
-        <v>342</v>
+        <v>664</v>
       </c>
       <c r="AK1" s="0" t="s">
-        <v>343</v>
+        <v>665</v>
       </c>
       <c r="AL1" s="0" t="s">
-        <v>344</v>
+        <v>666</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>284</v>
+        <v>606</v>
       </c>
       <c r="B2" s="0">
         <v>70518</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>294</v>
+        <v>616</v>
       </c>
       <c r="D2" s="0">
         <v>3</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>297</v>
+        <v>619</v>
       </c>
       <c r="F2" s="0">
         <v>527.33900000000006</v>
@@ -2176,19 +3142,19 @@
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>285</v>
+        <v>607</v>
       </c>
       <c r="B3" s="0">
         <v>70518</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>294</v>
+        <v>616</v>
       </c>
       <c r="D3" s="0">
         <v>3</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>298</v>
+        <v>620</v>
       </c>
       <c r="F3" s="0">
         <v>509.87200000000001</v>
@@ -2290,19 +3256,19 @@
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>285</v>
+        <v>607</v>
       </c>
       <c r="B4" s="0">
         <v>70518</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>294</v>
+        <v>616</v>
       </c>
       <c r="D4" s="0">
         <v>3</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>299</v>
+        <v>621</v>
       </c>
       <c r="F4" s="0">
         <v>414.42200000000003</v>
@@ -2404,19 +3370,19 @@
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>286</v>
+        <v>608</v>
       </c>
       <c r="B5" s="0">
         <v>70518</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>294</v>
+        <v>616</v>
       </c>
       <c r="D5" s="0">
         <v>3</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>300</v>
+        <v>622</v>
       </c>
       <c r="F5" s="0">
         <v>466.68799999999999</v>
@@ -2516,19 +3482,19 @@
     </row>
     <row r="6">
       <c r="A6" s="0" t="s">
-        <v>286</v>
+        <v>608</v>
       </c>
       <c r="B6" s="0">
         <v>50618</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>294</v>
+        <v>616</v>
       </c>
       <c r="D6" s="0">
         <v>1</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>301</v>
+        <v>623</v>
       </c>
       <c r="F6" s="0">
         <v>383.32900000000001</v>
@@ -2632,19 +3598,19 @@
     </row>
     <row r="7">
       <c r="A7" s="0" t="s">
-        <v>287</v>
+        <v>609</v>
       </c>
       <c r="B7" s="0">
         <v>50618</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>294</v>
+        <v>616</v>
       </c>
       <c r="D7" s="0">
         <v>1</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>302</v>
+        <v>624</v>
       </c>
       <c r="F7" s="0">
         <v>476.22300000000001</v>
@@ -2746,19 +3712,19 @@
     </row>
     <row r="8">
       <c r="A8" s="0" t="s">
-        <v>288</v>
+        <v>610</v>
       </c>
       <c r="B8" s="0">
         <v>310120</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>294</v>
+        <v>616</v>
       </c>
       <c r="D8" s="0">
         <v>3</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>303</v>
+        <v>625</v>
       </c>
       <c r="F8" s="0">
         <v>380.67500000000001</v>
@@ -2862,19 +3828,19 @@
     </row>
     <row r="9">
       <c r="A9" s="0" t="s">
-        <v>288</v>
+        <v>610</v>
       </c>
       <c r="B9" s="0">
         <v>260420</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>294</v>
+        <v>616</v>
       </c>
       <c r="D9" s="0">
         <v>2</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>304</v>
+        <v>626</v>
       </c>
       <c r="F9" s="0">
         <v>373.99900000000002</v>
@@ -2976,19 +3942,19 @@
     </row>
     <row r="10">
       <c r="A10" s="0" t="s">
-        <v>288</v>
+        <v>610</v>
       </c>
       <c r="B10" s="0">
         <v>260420</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>294</v>
+        <v>616</v>
       </c>
       <c r="D10" s="0">
         <v>2</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>305</v>
+        <v>627</v>
       </c>
       <c r="F10" s="0">
         <v>384.10599999999999</v>
@@ -3090,19 +4056,19 @@
     </row>
     <row r="11">
       <c r="A11" s="0" t="s">
-        <v>288</v>
+        <v>610</v>
       </c>
       <c r="B11" s="0">
         <v>280420</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>294</v>
+        <v>616</v>
       </c>
       <c r="D11" s="0">
         <v>2</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>306</v>
+        <v>628</v>
       </c>
       <c r="F11" s="0">
         <v>319.63099999999997</v>
@@ -3204,19 +4170,19 @@
     </row>
     <row r="12">
       <c r="A12" s="0" t="s">
-        <v>289</v>
+        <v>611</v>
       </c>
       <c r="B12" s="0">
         <v>280420</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>294</v>
+        <v>616</v>
       </c>
       <c r="D12" s="0">
         <v>3</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>307</v>
+        <v>629</v>
       </c>
       <c r="F12" s="0">
         <v>375.012</v>
@@ -3318,19 +4284,19 @@
     </row>
     <row r="13">
       <c r="A13" s="0" t="s">
-        <v>289</v>
+        <v>611</v>
       </c>
       <c r="B13" s="0">
         <v>290420</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>294</v>
+        <v>616</v>
       </c>
       <c r="D13" s="0">
         <v>2</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>308</v>
+        <v>630</v>
       </c>
       <c r="F13" s="0">
         <v>381.83600000000001</v>
@@ -3432,19 +4398,19 @@
     </row>
     <row r="14">
       <c r="A14" s="0" t="s">
-        <v>289</v>
+        <v>611</v>
       </c>
       <c r="B14" s="0">
         <v>20520</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>294</v>
+        <v>616</v>
       </c>
       <c r="D14" s="0">
         <v>3</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>309</v>
+        <v>631</v>
       </c>
       <c r="F14" s="0">
         <v>426.51900000000001</v>
@@ -3546,19 +4512,19 @@
     </row>
     <row r="15">
       <c r="A15" s="0" t="s">
-        <v>290</v>
+        <v>612</v>
       </c>
       <c r="B15" s="0">
         <v>20520</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>294</v>
+        <v>616</v>
       </c>
       <c r="D15" s="0">
         <v>3</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>310</v>
+        <v>632</v>
       </c>
       <c r="F15" s="0">
         <v>397.04599999999999</v>
@@ -3660,19 +4626,19 @@
     </row>
     <row r="16">
       <c r="A16" s="0" t="s">
-        <v>291</v>
+        <v>613</v>
       </c>
       <c r="B16" s="0">
         <v>30221</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>294</v>
+        <v>616</v>
       </c>
       <c r="D16" s="0">
         <v>2</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>311</v>
+        <v>633</v>
       </c>
       <c r="F16" s="0">
         <v>378.37099999999998</v>
@@ -3777,177 +4743,177 @@
   <dimension ref="A1:AL16"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="5.48828125" customWidth="true"/>
-    <col min="2" max="2" width="7.15625" customWidth="true"/>
-    <col min="3" max="3" width="10.37890625" customWidth="true"/>
-    <col min="4" max="4" width="4.82421875" customWidth="true"/>
-    <col min="5" max="5" width="3.82421875" customWidth="true"/>
+    <col min="1" max="1" width="5.85546875" customWidth="true"/>
+    <col min="2" max="2" width="7.140625" customWidth="true"/>
+    <col min="3" max="3" width="11.42578125" customWidth="true"/>
+    <col min="4" max="4" width="5.28515625" customWidth="true"/>
+    <col min="5" max="5" width="3.85546875" customWidth="true"/>
     <col min="6" max="6" width="7.7109375" customWidth="true"/>
-    <col min="7" max="7" width="10.15625" customWidth="true"/>
-    <col min="8" max="8" width="7.37890625" customWidth="true"/>
-    <col min="9" max="9" width="9.15625" customWidth="true"/>
+    <col min="7" max="7" width="10.85546875" customWidth="true"/>
+    <col min="8" max="8" width="8" customWidth="true"/>
+    <col min="9" max="9" width="10.140625" customWidth="true"/>
     <col min="10" max="10" width="7.7109375" customWidth="true"/>
-    <col min="11" max="11" width="8.7109375" customWidth="true"/>
-    <col min="12" max="12" width="9.26953125" customWidth="true"/>
+    <col min="11" max="11" width="9.42578125" customWidth="true"/>
+    <col min="12" max="12" width="10" customWidth="true"/>
     <col min="13" max="13" width="7.7109375" customWidth="true"/>
     <col min="14" max="14" width="6.7109375" customWidth="true"/>
-    <col min="15" max="15" width="4.37890625" customWidth="true"/>
-    <col min="16" max="16" width="7.93359375" customWidth="true"/>
-    <col min="17" max="17" width="7.82421875" customWidth="true"/>
+    <col min="15" max="15" width="4.7109375" customWidth="true"/>
+    <col min="16" max="16" width="8.140625" customWidth="true"/>
+    <col min="17" max="17" width="8.140625" customWidth="true"/>
     <col min="18" max="18" width="6.7109375" customWidth="true"/>
-    <col min="19" max="19" width="9.37890625" customWidth="true"/>
-    <col min="20" max="20" width="7.37890625" customWidth="true"/>
+    <col min="19" max="19" width="10" customWidth="true"/>
+    <col min="20" max="20" width="8.28515625" customWidth="true"/>
     <col min="21" max="21" width="11.7109375" customWidth="true"/>
-    <col min="22" max="22" width="8.046875" customWidth="true"/>
+    <col min="22" max="22" width="8.85546875" customWidth="true"/>
     <col min="23" max="23" width="11.7109375" customWidth="true"/>
-    <col min="24" max="24" width="10.37890625" customWidth="true"/>
-    <col min="25" max="25" width="11.7109375" customWidth="true"/>
+    <col min="24" max="24" width="10.42578125" customWidth="true"/>
+    <col min="25" max="25" width="12.42578125" customWidth="true"/>
     <col min="26" max="26" width="11.7109375" customWidth="true"/>
     <col min="27" max="27" width="13.7109375" customWidth="true"/>
     <col min="28" max="28" width="12.7109375" customWidth="true"/>
-    <col min="29" max="29" width="10.26953125" customWidth="true"/>
-    <col min="30" max="30" width="11.48828125" customWidth="true"/>
+    <col min="29" max="29" width="11.28515625" customWidth="true"/>
+    <col min="30" max="30" width="13" customWidth="true"/>
     <col min="31" max="31" width="12.7109375" customWidth="true"/>
-    <col min="32" max="32" width="9.15625" customWidth="true"/>
-    <col min="33" max="33" width="7.93359375" customWidth="true"/>
+    <col min="32" max="32" width="10" customWidth="true"/>
+    <col min="33" max="33" width="8.7109375" customWidth="true"/>
     <col min="34" max="34" width="7.7109375" customWidth="true"/>
     <col min="35" max="35" width="11.7109375" customWidth="true"/>
-    <col min="36" max="36" width="3.7109375" customWidth="true"/>
+    <col min="36" max="36" width="4" customWidth="true"/>
     <col min="37" max="37" width="7.7109375" customWidth="true"/>
-    <col min="38" max="38" width="13.7109375" customWidth="true"/>
+    <col min="38" max="38" width="15" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>345</v>
+        <v>667</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>356</v>
+        <v>678</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>357</v>
+        <v>679</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>359</v>
+        <v>681</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>360</v>
+        <v>682</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>376</v>
+        <v>698</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>377</v>
+        <v>699</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>378</v>
+        <v>700</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>379</v>
+        <v>701</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>380</v>
+        <v>702</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>381</v>
+        <v>703</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>382</v>
+        <v>704</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>383</v>
+        <v>705</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>384</v>
+        <v>706</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>385</v>
+        <v>707</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>386</v>
+        <v>708</v>
       </c>
       <c r="Q1" s="0" t="s">
-        <v>387</v>
+        <v>709</v>
       </c>
       <c r="R1" s="0" t="s">
-        <v>388</v>
+        <v>710</v>
       </c>
       <c r="S1" s="0" t="s">
-        <v>389</v>
+        <v>711</v>
       </c>
       <c r="T1" s="0" t="s">
-        <v>390</v>
+        <v>712</v>
       </c>
       <c r="U1" s="0" t="s">
-        <v>391</v>
+        <v>713</v>
       </c>
       <c r="V1" s="0" t="s">
-        <v>392</v>
+        <v>714</v>
       </c>
       <c r="W1" s="0" t="s">
-        <v>393</v>
+        <v>715</v>
       </c>
       <c r="X1" s="0" t="s">
-        <v>394</v>
+        <v>716</v>
       </c>
       <c r="Y1" s="0" t="s">
-        <v>395</v>
+        <v>717</v>
       </c>
       <c r="Z1" s="0" t="s">
-        <v>396</v>
+        <v>718</v>
       </c>
       <c r="AA1" s="0" t="s">
-        <v>397</v>
+        <v>719</v>
       </c>
       <c r="AB1" s="0" t="s">
-        <v>398</v>
+        <v>720</v>
       </c>
       <c r="AC1" s="0" t="s">
-        <v>399</v>
+        <v>721</v>
       </c>
       <c r="AD1" s="0" t="s">
-        <v>400</v>
+        <v>722</v>
       </c>
       <c r="AE1" s="0" t="s">
-        <v>401</v>
+        <v>723</v>
       </c>
       <c r="AF1" s="0" t="s">
-        <v>402</v>
+        <v>724</v>
       </c>
       <c r="AG1" s="0" t="s">
-        <v>403</v>
+        <v>725</v>
       </c>
       <c r="AH1" s="0" t="s">
-        <v>404</v>
+        <v>726</v>
       </c>
       <c r="AI1" s="0" t="s">
-        <v>405</v>
+        <v>727</v>
       </c>
       <c r="AJ1" s="0" t="s">
-        <v>406</v>
+        <v>728</v>
       </c>
       <c r="AK1" s="0" t="s">
-        <v>407</v>
+        <v>729</v>
       </c>
       <c r="AL1" s="0" t="s">
-        <v>408</v>
+        <v>730</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>346</v>
+        <v>668</v>
       </c>
       <c r="B2" s="0">
         <v>250320</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>358</v>
+        <v>680</v>
       </c>
       <c r="D2" s="0">
         <v>2</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>361</v>
+        <v>683</v>
       </c>
       <c r="F2" s="0">
         <v>428.44900000000001</v>
@@ -4051,19 +5017,19 @@
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>347</v>
+        <v>669</v>
       </c>
       <c r="B3" s="0">
         <v>260320</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>358</v>
+        <v>680</v>
       </c>
       <c r="D3" s="0">
         <v>2</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>362</v>
+        <v>684</v>
       </c>
       <c r="F3" s="0">
         <v>465.96699999999998</v>
@@ -4165,19 +5131,19 @@
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>348</v>
+        <v>670</v>
       </c>
       <c r="B4" s="0">
         <v>260320</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>358</v>
+        <v>680</v>
       </c>
       <c r="D4" s="0">
         <v>2</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>363</v>
+        <v>685</v>
       </c>
       <c r="F4" s="0">
         <v>514.60299999999995</v>
@@ -4275,19 +5241,19 @@
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>348</v>
+        <v>670</v>
       </c>
       <c r="B5" s="0">
         <v>140520</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>358</v>
+        <v>680</v>
       </c>
       <c r="D5" s="0">
         <v>2</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>364</v>
+        <v>686</v>
       </c>
       <c r="F5" s="0">
         <v>490.94</v>
@@ -4383,19 +5349,19 @@
     </row>
     <row r="6">
       <c r="A6" s="0" t="s">
-        <v>349</v>
+        <v>671</v>
       </c>
       <c r="B6" s="0">
         <v>150520</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>358</v>
+        <v>680</v>
       </c>
       <c r="D6" s="0">
         <v>1</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>365</v>
+        <v>687</v>
       </c>
       <c r="F6" s="0">
         <v>515.92899999999997</v>
@@ -4497,19 +5463,19 @@
     </row>
     <row r="7">
       <c r="A7" s="0" t="s">
-        <v>350</v>
+        <v>672</v>
       </c>
       <c r="B7" s="0">
         <v>150520</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>358</v>
+        <v>680</v>
       </c>
       <c r="D7" s="0">
         <v>1</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>366</v>
+        <v>688</v>
       </c>
       <c r="F7" s="0">
         <v>500.041</v>
@@ -4607,19 +5573,19 @@
     </row>
     <row r="8">
       <c r="A8" s="0" t="s">
-        <v>350</v>
+        <v>672</v>
       </c>
       <c r="B8" s="0">
         <v>190520</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>358</v>
+        <v>680</v>
       </c>
       <c r="D8" s="0">
         <v>1</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>367</v>
+        <v>689</v>
       </c>
       <c r="F8" s="0">
         <v>475.017</v>
@@ -4723,19 +5689,19 @@
     </row>
     <row r="9">
       <c r="A9" s="0" t="s">
-        <v>350</v>
+        <v>672</v>
       </c>
       <c r="B9" s="0">
         <v>190520</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>358</v>
+        <v>680</v>
       </c>
       <c r="D9" s="0">
         <v>1</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>368</v>
+        <v>690</v>
       </c>
       <c r="F9" s="0">
         <v>570.43799999999999</v>
@@ -4837,19 +5803,19 @@
     </row>
     <row r="10">
       <c r="A10" s="0" t="s">
-        <v>351</v>
+        <v>673</v>
       </c>
       <c r="B10" s="0">
         <v>200520</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>358</v>
+        <v>680</v>
       </c>
       <c r="D10" s="0">
         <v>2</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>369</v>
+        <v>691</v>
       </c>
       <c r="F10" s="0">
         <v>512.58900000000006</v>
@@ -4951,19 +5917,19 @@
     </row>
     <row r="11">
       <c r="A11" s="0" t="s">
-        <v>352</v>
+        <v>674</v>
       </c>
       <c r="B11" s="0">
         <v>210520</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>358</v>
+        <v>680</v>
       </c>
       <c r="D11" s="0">
         <v>1</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>370</v>
+        <v>692</v>
       </c>
       <c r="F11" s="0">
         <v>482.98500000000001</v>
@@ -5065,19 +6031,19 @@
     </row>
     <row r="12">
       <c r="A12" s="0" t="s">
-        <v>353</v>
+        <v>675</v>
       </c>
       <c r="B12" s="0">
         <v>210520</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>358</v>
+        <v>680</v>
       </c>
       <c r="D12" s="0">
         <v>1</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>371</v>
+        <v>693</v>
       </c>
       <c r="F12" s="0">
         <v>510.274</v>
@@ -5179,19 +6145,19 @@
     </row>
     <row r="13">
       <c r="A13" s="0" t="s">
-        <v>353</v>
+        <v>675</v>
       </c>
       <c r="B13" s="0">
         <v>210520</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>358</v>
+        <v>680</v>
       </c>
       <c r="D13" s="0">
         <v>2</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>372</v>
+        <v>694</v>
       </c>
       <c r="F13" s="0">
         <v>570.12</v>
@@ -5293,19 +6259,19 @@
     </row>
     <row r="14">
       <c r="A14" s="0" t="s">
-        <v>354</v>
+        <v>676</v>
       </c>
       <c r="B14" s="0">
         <v>240520</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>358</v>
+        <v>680</v>
       </c>
       <c r="D14" s="0">
         <v>1</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>373</v>
+        <v>695</v>
       </c>
       <c r="F14" s="0">
         <v>352.471</v>
@@ -5409,19 +6375,19 @@
     </row>
     <row r="15">
       <c r="A15" s="0" t="s">
-        <v>355</v>
+        <v>677</v>
       </c>
       <c r="B15" s="0">
         <v>240520</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>358</v>
+        <v>680</v>
       </c>
       <c r="D15" s="0">
         <v>2</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>374</v>
+        <v>696</v>
       </c>
       <c r="F15" s="0">
         <v>432.50099999999998</v>
@@ -5523,19 +6489,19 @@
     </row>
     <row r="16">
       <c r="A16" s="0" t="s">
-        <v>355</v>
+        <v>677</v>
       </c>
       <c r="B16" s="0">
         <v>240520</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>358</v>
+        <v>680</v>
       </c>
       <c r="D16" s="0">
         <v>2</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>375</v>
+        <v>697</v>
       </c>
       <c r="F16" s="0">
         <v>420.47899999999998</v>
@@ -5644,177 +6610,177 @@
   <dimension ref="A1:AL6"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="5.48828125" customWidth="true"/>
-    <col min="2" max="2" width="7.15625" customWidth="true"/>
-    <col min="3" max="3" width="10.37890625" customWidth="true"/>
-    <col min="4" max="4" width="4.82421875" customWidth="true"/>
-    <col min="5" max="5" width="3.82421875" customWidth="true"/>
+    <col min="1" max="1" width="5.85546875" customWidth="true"/>
+    <col min="2" max="2" width="7.140625" customWidth="true"/>
+    <col min="3" max="3" width="11.42578125" customWidth="true"/>
+    <col min="4" max="4" width="5.28515625" customWidth="true"/>
+    <col min="5" max="5" width="3.85546875" customWidth="true"/>
     <col min="6" max="6" width="7.7109375" customWidth="true"/>
-    <col min="7" max="7" width="10.15625" customWidth="true"/>
-    <col min="8" max="8" width="7.37890625" customWidth="true"/>
-    <col min="9" max="9" width="9.15625" customWidth="true"/>
+    <col min="7" max="7" width="10.85546875" customWidth="true"/>
+    <col min="8" max="8" width="8" customWidth="true"/>
+    <col min="9" max="9" width="10.140625" customWidth="true"/>
     <col min="10" max="10" width="7.7109375" customWidth="true"/>
-    <col min="11" max="11" width="8.7109375" customWidth="true"/>
-    <col min="12" max="12" width="9.26953125" customWidth="true"/>
+    <col min="11" max="11" width="9.42578125" customWidth="true"/>
+    <col min="12" max="12" width="10" customWidth="true"/>
     <col min="13" max="13" width="7.7109375" customWidth="true"/>
     <col min="14" max="14" width="7.7109375" customWidth="true"/>
-    <col min="15" max="15" width="4.37890625" customWidth="true"/>
-    <col min="16" max="16" width="7.93359375" customWidth="true"/>
-    <col min="17" max="17" width="7.82421875" customWidth="true"/>
+    <col min="15" max="15" width="4.7109375" customWidth="true"/>
+    <col min="16" max="16" width="8.140625" customWidth="true"/>
+    <col min="17" max="17" width="8.140625" customWidth="true"/>
     <col min="18" max="18" width="6.7109375" customWidth="true"/>
-    <col min="19" max="19" width="9.37890625" customWidth="true"/>
-    <col min="20" max="20" width="7.37890625" customWidth="true"/>
+    <col min="19" max="19" width="10" customWidth="true"/>
+    <col min="20" max="20" width="8.28515625" customWidth="true"/>
     <col min="21" max="21" width="11.7109375" customWidth="true"/>
-    <col min="22" max="22" width="8.7109375" customWidth="true"/>
+    <col min="22" max="22" width="8.85546875" customWidth="true"/>
     <col min="23" max="23" width="11.7109375" customWidth="true"/>
-    <col min="24" max="24" width="10.37890625" customWidth="true"/>
-    <col min="25" max="25" width="11.7109375" customWidth="true"/>
+    <col min="24" max="24" width="10.42578125" customWidth="true"/>
+    <col min="25" max="25" width="12.42578125" customWidth="true"/>
     <col min="26" max="26" width="11.7109375" customWidth="true"/>
     <col min="27" max="27" width="13.7109375" customWidth="true"/>
     <col min="28" max="28" width="12.7109375" customWidth="true"/>
-    <col min="29" max="29" width="10.26953125" customWidth="true"/>
-    <col min="30" max="30" width="11.48828125" customWidth="true"/>
+    <col min="29" max="29" width="11.28515625" customWidth="true"/>
+    <col min="30" max="30" width="13" customWidth="true"/>
     <col min="31" max="31" width="11.7109375" customWidth="true"/>
-    <col min="32" max="32" width="9.15625" customWidth="true"/>
-    <col min="33" max="33" width="7.93359375" customWidth="true"/>
+    <col min="32" max="32" width="10" customWidth="true"/>
+    <col min="33" max="33" width="8.7109375" customWidth="true"/>
     <col min="34" max="34" width="7.7109375" customWidth="true"/>
     <col min="35" max="35" width="11.7109375" customWidth="true"/>
     <col min="36" max="36" width="11.7109375" customWidth="true"/>
     <col min="37" max="37" width="6.7109375" customWidth="true"/>
-    <col min="38" max="38" width="13.7109375" customWidth="true"/>
+    <col min="38" max="38" width="15" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>409</v>
+        <v>731</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>413</v>
+        <v>735</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>414</v>
+        <v>736</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>416</v>
+        <v>738</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>417</v>
+        <v>739</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>422</v>
+        <v>744</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>423</v>
+        <v>745</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>424</v>
+        <v>746</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>425</v>
+        <v>747</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>426</v>
+        <v>748</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>427</v>
+        <v>749</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>428</v>
+        <v>750</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>429</v>
+        <v>751</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>430</v>
+        <v>752</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>431</v>
+        <v>753</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>432</v>
+        <v>754</v>
       </c>
       <c r="Q1" s="0" t="s">
-        <v>433</v>
+        <v>755</v>
       </c>
       <c r="R1" s="0" t="s">
-        <v>434</v>
+        <v>756</v>
       </c>
       <c r="S1" s="0" t="s">
-        <v>435</v>
+        <v>757</v>
       </c>
       <c r="T1" s="0" t="s">
-        <v>436</v>
+        <v>758</v>
       </c>
       <c r="U1" s="0" t="s">
-        <v>437</v>
+        <v>759</v>
       </c>
       <c r="V1" s="0" t="s">
-        <v>438</v>
+        <v>760</v>
       </c>
       <c r="W1" s="0" t="s">
-        <v>439</v>
+        <v>761</v>
       </c>
       <c r="X1" s="0" t="s">
-        <v>440</v>
+        <v>762</v>
       </c>
       <c r="Y1" s="0" t="s">
-        <v>441</v>
+        <v>763</v>
       </c>
       <c r="Z1" s="0" t="s">
-        <v>442</v>
+        <v>764</v>
       </c>
       <c r="AA1" s="0" t="s">
-        <v>443</v>
+        <v>765</v>
       </c>
       <c r="AB1" s="0" t="s">
-        <v>444</v>
+        <v>766</v>
       </c>
       <c r="AC1" s="0" t="s">
-        <v>445</v>
+        <v>767</v>
       </c>
       <c r="AD1" s="0" t="s">
-        <v>446</v>
+        <v>768</v>
       </c>
       <c r="AE1" s="0" t="s">
-        <v>447</v>
+        <v>769</v>
       </c>
       <c r="AF1" s="0" t="s">
-        <v>448</v>
+        <v>770</v>
       </c>
       <c r="AG1" s="0" t="s">
-        <v>449</v>
+        <v>771</v>
       </c>
       <c r="AH1" s="0" t="s">
-        <v>450</v>
+        <v>772</v>
       </c>
       <c r="AI1" s="0" t="s">
-        <v>451</v>
+        <v>773</v>
       </c>
       <c r="AJ1" s="0" t="s">
-        <v>452</v>
+        <v>774</v>
       </c>
       <c r="AK1" s="0" t="s">
-        <v>453</v>
+        <v>775</v>
       </c>
       <c r="AL1" s="0" t="s">
-        <v>454</v>
+        <v>776</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>410</v>
+        <v>732</v>
       </c>
       <c r="B2" s="0">
         <v>21018</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>415</v>
+        <v>737</v>
       </c>
       <c r="D2" s="0">
         <v>2</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>418</v>
+        <v>740</v>
       </c>
       <c r="F2" s="0">
         <v>363.99400000000003</v>
@@ -5916,19 +6882,19 @@
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>411</v>
+        <v>733</v>
       </c>
       <c r="B3" s="0">
         <v>160519</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>415</v>
+        <v>737</v>
       </c>
       <c r="D3" s="0">
         <v>1</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>418</v>
+        <v>740</v>
       </c>
       <c r="F3" s="0">
         <v>407.608</v>
@@ -6030,19 +6996,19 @@
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>412</v>
+        <v>734</v>
       </c>
       <c r="B4" s="0">
         <v>160519</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>415</v>
+        <v>737</v>
       </c>
       <c r="D4" s="0">
         <v>3</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>419</v>
+        <v>741</v>
       </c>
       <c r="F4" s="0">
         <v>503.45100000000002</v>
@@ -6148,13 +7114,13 @@
         <v>21018</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>415</v>
+        <v>737</v>
       </c>
       <c r="D5" s="0">
         <v>2</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>420</v>
+        <v>742</v>
       </c>
       <c r="F5" s="0">
         <v>342.95400000000001</v>
@@ -6260,13 +7226,13 @@
         <v>270319</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>415</v>
+        <v>737</v>
       </c>
       <c r="D6" s="0">
         <v>3</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>421</v>
+        <v>743</v>
       </c>
       <c r="F6" s="0">
         <v>553.14999999999998</v>
@@ -6375,177 +7341,177 @@
   <dimension ref="A1:AL6"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="5.48828125" customWidth="true"/>
-    <col min="2" max="2" width="7.15625" customWidth="true"/>
-    <col min="3" max="3" width="10.37890625" customWidth="true"/>
-    <col min="4" max="4" width="4.82421875" customWidth="true"/>
-    <col min="5" max="5" width="3.82421875" customWidth="true"/>
+    <col min="1" max="1" width="5.85546875" customWidth="true"/>
+    <col min="2" max="2" width="7.140625" customWidth="true"/>
+    <col min="3" max="3" width="11.42578125" customWidth="true"/>
+    <col min="4" max="4" width="5.28515625" customWidth="true"/>
+    <col min="5" max="5" width="3.85546875" customWidth="true"/>
     <col min="6" max="6" width="7.7109375" customWidth="true"/>
-    <col min="7" max="7" width="10.15625" customWidth="true"/>
-    <col min="8" max="8" width="7.37890625" customWidth="true"/>
-    <col min="9" max="9" width="9.15625" customWidth="true"/>
+    <col min="7" max="7" width="10.85546875" customWidth="true"/>
+    <col min="8" max="8" width="8" customWidth="true"/>
+    <col min="9" max="9" width="10.140625" customWidth="true"/>
     <col min="10" max="10" width="7.7109375" customWidth="true"/>
-    <col min="11" max="11" width="8.7109375" customWidth="true"/>
-    <col min="12" max="12" width="9.26953125" customWidth="true"/>
+    <col min="11" max="11" width="9.42578125" customWidth="true"/>
+    <col min="12" max="12" width="10" customWidth="true"/>
     <col min="13" max="13" width="7.7109375" customWidth="true"/>
     <col min="14" max="14" width="7.7109375" customWidth="true"/>
-    <col min="15" max="15" width="4.37890625" customWidth="true"/>
-    <col min="16" max="16" width="7.93359375" customWidth="true"/>
-    <col min="17" max="17" width="7.82421875" customWidth="true"/>
+    <col min="15" max="15" width="4.7109375" customWidth="true"/>
+    <col min="16" max="16" width="8.140625" customWidth="true"/>
+    <col min="17" max="17" width="8.140625" customWidth="true"/>
     <col min="18" max="18" width="6.7109375" customWidth="true"/>
-    <col min="19" max="19" width="9.37890625" customWidth="true"/>
-    <col min="20" max="20" width="7.37890625" customWidth="true"/>
+    <col min="19" max="19" width="10" customWidth="true"/>
+    <col min="20" max="20" width="8.28515625" customWidth="true"/>
     <col min="21" max="21" width="11.7109375" customWidth="true"/>
-    <col min="22" max="22" width="8.046875" customWidth="true"/>
+    <col min="22" max="22" width="8.85546875" customWidth="true"/>
     <col min="23" max="23" width="11.7109375" customWidth="true"/>
-    <col min="24" max="24" width="9.37890625" customWidth="true"/>
-    <col min="25" max="25" width="11.7109375" customWidth="true"/>
+    <col min="24" max="24" width="9.42578125" customWidth="true"/>
+    <col min="25" max="25" width="12.42578125" customWidth="true"/>
     <col min="26" max="26" width="11.7109375" customWidth="true"/>
     <col min="27" max="27" width="13.7109375" customWidth="true"/>
     <col min="28" max="28" width="12.7109375" customWidth="true"/>
-    <col min="29" max="29" width="10.26953125" customWidth="true"/>
-    <col min="30" max="30" width="11.48828125" customWidth="true"/>
+    <col min="29" max="29" width="11.28515625" customWidth="true"/>
+    <col min="30" max="30" width="13" customWidth="true"/>
     <col min="31" max="31" width="12.7109375" customWidth="true"/>
     <col min="32" max="32" width="10.7109375" customWidth="true"/>
     <col min="33" max="33" width="8.7109375" customWidth="true"/>
     <col min="34" max="34" width="7.7109375" customWidth="true"/>
     <col min="35" max="35" width="11.7109375" customWidth="true"/>
-    <col min="36" max="36" width="3.7109375" customWidth="true"/>
-    <col min="37" max="37" width="7.37890625" customWidth="true"/>
-    <col min="38" max="38" width="13.7109375" customWidth="true"/>
+    <col min="36" max="36" width="4" customWidth="true"/>
+    <col min="37" max="37" width="7.42578125" customWidth="true"/>
+    <col min="38" max="38" width="15" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>455</v>
+        <v>777</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>457</v>
+        <v>779</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>458</v>
+        <v>780</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>460</v>
+        <v>782</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>461</v>
+        <v>783</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>467</v>
+        <v>789</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>468</v>
+        <v>790</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>469</v>
+        <v>791</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>470</v>
+        <v>792</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>471</v>
+        <v>793</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>472</v>
+        <v>794</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>473</v>
+        <v>795</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>474</v>
+        <v>796</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>475</v>
+        <v>797</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>476</v>
+        <v>798</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>477</v>
+        <v>799</v>
       </c>
       <c r="Q1" s="0" t="s">
-        <v>478</v>
+        <v>800</v>
       </c>
       <c r="R1" s="0" t="s">
-        <v>479</v>
+        <v>801</v>
       </c>
       <c r="S1" s="0" t="s">
-        <v>480</v>
+        <v>802</v>
       </c>
       <c r="T1" s="0" t="s">
-        <v>481</v>
+        <v>803</v>
       </c>
       <c r="U1" s="0" t="s">
-        <v>482</v>
+        <v>804</v>
       </c>
       <c r="V1" s="0" t="s">
-        <v>483</v>
+        <v>805</v>
       </c>
       <c r="W1" s="0" t="s">
-        <v>484</v>
+        <v>806</v>
       </c>
       <c r="X1" s="0" t="s">
-        <v>485</v>
+        <v>807</v>
       </c>
       <c r="Y1" s="0" t="s">
-        <v>486</v>
+        <v>808</v>
       </c>
       <c r="Z1" s="0" t="s">
-        <v>487</v>
+        <v>809</v>
       </c>
       <c r="AA1" s="0" t="s">
-        <v>488</v>
+        <v>810</v>
       </c>
       <c r="AB1" s="0" t="s">
-        <v>489</v>
+        <v>811</v>
       </c>
       <c r="AC1" s="0" t="s">
-        <v>490</v>
+        <v>812</v>
       </c>
       <c r="AD1" s="0" t="s">
-        <v>491</v>
+        <v>813</v>
       </c>
       <c r="AE1" s="0" t="s">
-        <v>492</v>
+        <v>814</v>
       </c>
       <c r="AF1" s="0" t="s">
-        <v>493</v>
+        <v>815</v>
       </c>
       <c r="AG1" s="0" t="s">
-        <v>494</v>
+        <v>816</v>
       </c>
       <c r="AH1" s="0" t="s">
-        <v>495</v>
+        <v>817</v>
       </c>
       <c r="AI1" s="0" t="s">
-        <v>496</v>
+        <v>818</v>
       </c>
       <c r="AJ1" s="0" t="s">
-        <v>497</v>
+        <v>819</v>
       </c>
       <c r="AK1" s="0" t="s">
-        <v>498</v>
+        <v>820</v>
       </c>
       <c r="AL1" s="0" t="s">
-        <v>499</v>
+        <v>821</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>456</v>
+        <v>778</v>
       </c>
       <c r="B2" s="0">
         <v>30518</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>459</v>
+        <v>781</v>
       </c>
       <c r="D2" s="0">
         <v>2</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>462</v>
+        <v>784</v>
       </c>
       <c r="F2" s="0">
         <v>590.19000000000005</v>
@@ -6649,19 +7615,19 @@
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>456</v>
+        <v>778</v>
       </c>
       <c r="B3" s="0">
         <v>41220</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>459</v>
+        <v>781</v>
       </c>
       <c r="D3" s="0">
         <v>2</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>463</v>
+        <v>785</v>
       </c>
       <c r="F3" s="0">
         <v>527.303</v>
@@ -6763,19 +7729,19 @@
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>456</v>
+        <v>778</v>
       </c>
       <c r="B4" s="0">
         <v>190121</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>459</v>
+        <v>781</v>
       </c>
       <c r="D4" s="0">
         <v>2</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>464</v>
+        <v>786</v>
       </c>
       <c r="F4" s="0">
         <v>531.99300000000005</v>
@@ -6877,19 +7843,19 @@
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>456</v>
+        <v>778</v>
       </c>
       <c r="B5" s="0">
         <v>190121</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>459</v>
+        <v>781</v>
       </c>
       <c r="D5" s="0">
         <v>3</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>465</v>
+        <v>787</v>
       </c>
       <c r="F5" s="0">
         <v>406.07999999999998</v>
@@ -6991,19 +7957,19 @@
     </row>
     <row r="6">
       <c r="A6" s="0" t="s">
-        <v>456</v>
+        <v>778</v>
       </c>
       <c r="B6" s="0">
         <v>190121</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>459</v>
+        <v>781</v>
       </c>
       <c r="D6" s="0">
         <v>3</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>466</v>
+        <v>788</v>
       </c>
       <c r="F6" s="0">
         <v>363.67099999999999</v>
@@ -7112,177 +8078,177 @@
   <dimension ref="A1:AL7"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="5.48828125" customWidth="true"/>
-    <col min="2" max="2" width="7.15625" customWidth="true"/>
-    <col min="3" max="3" width="10.37890625" customWidth="true"/>
-    <col min="4" max="4" width="4.82421875" customWidth="true"/>
-    <col min="5" max="5" width="3.82421875" customWidth="true"/>
+    <col min="1" max="1" width="5.85546875" customWidth="true"/>
+    <col min="2" max="2" width="7.140625" customWidth="true"/>
+    <col min="3" max="3" width="11.42578125" customWidth="true"/>
+    <col min="4" max="4" width="5.28515625" customWidth="true"/>
+    <col min="5" max="5" width="3.85546875" customWidth="true"/>
     <col min="6" max="6" width="7.7109375" customWidth="true"/>
-    <col min="7" max="7" width="10.15625" customWidth="true"/>
-    <col min="8" max="8" width="7.37890625" customWidth="true"/>
-    <col min="9" max="9" width="9.15625" customWidth="true"/>
+    <col min="7" max="7" width="10.85546875" customWidth="true"/>
+    <col min="8" max="8" width="8" customWidth="true"/>
+    <col min="9" max="9" width="10.140625" customWidth="true"/>
     <col min="10" max="10" width="7.7109375" customWidth="true"/>
-    <col min="11" max="11" width="8.7109375" customWidth="true"/>
-    <col min="12" max="12" width="9.26953125" customWidth="true"/>
+    <col min="11" max="11" width="9.42578125" customWidth="true"/>
+    <col min="12" max="12" width="10" customWidth="true"/>
     <col min="13" max="13" width="6.7109375" customWidth="true"/>
     <col min="14" max="14" width="6.7109375" customWidth="true"/>
-    <col min="15" max="15" width="4.37890625" customWidth="true"/>
-    <col min="16" max="16" width="7.93359375" customWidth="true"/>
-    <col min="17" max="17" width="7.82421875" customWidth="true"/>
+    <col min="15" max="15" width="4.7109375" customWidth="true"/>
+    <col min="16" max="16" width="8.140625" customWidth="true"/>
+    <col min="17" max="17" width="8.140625" customWidth="true"/>
     <col min="18" max="18" width="6.7109375" customWidth="true"/>
-    <col min="19" max="19" width="9.37890625" customWidth="true"/>
-    <col min="20" max="20" width="7.37890625" customWidth="true"/>
+    <col min="19" max="19" width="10" customWidth="true"/>
+    <col min="20" max="20" width="8.28515625" customWidth="true"/>
     <col min="21" max="21" width="11.7109375" customWidth="true"/>
-    <col min="22" max="22" width="8.046875" customWidth="true"/>
+    <col min="22" max="22" width="8.85546875" customWidth="true"/>
     <col min="23" max="23" width="11.7109375" customWidth="true"/>
-    <col min="24" max="24" width="10.37890625" customWidth="true"/>
-    <col min="25" max="25" width="11.7109375" customWidth="true"/>
+    <col min="24" max="24" width="10.42578125" customWidth="true"/>
+    <col min="25" max="25" width="12.42578125" customWidth="true"/>
     <col min="26" max="26" width="11.7109375" customWidth="true"/>
     <col min="27" max="27" width="13.7109375" customWidth="true"/>
     <col min="28" max="28" width="12.7109375" customWidth="true"/>
-    <col min="29" max="29" width="10.26953125" customWidth="true"/>
-    <col min="30" max="30" width="11.48828125" customWidth="true"/>
+    <col min="29" max="29" width="11.28515625" customWidth="true"/>
+    <col min="30" max="30" width="13" customWidth="true"/>
     <col min="31" max="31" width="12.7109375" customWidth="true"/>
-    <col min="32" max="32" width="9.15625" customWidth="true"/>
-    <col min="33" max="33" width="7.93359375" customWidth="true"/>
+    <col min="32" max="32" width="10" customWidth="true"/>
+    <col min="33" max="33" width="8.7109375" customWidth="true"/>
     <col min="34" max="34" width="7.7109375" customWidth="true"/>
     <col min="35" max="35" width="11.7109375" customWidth="true"/>
-    <col min="36" max="36" width="3.7109375" customWidth="true"/>
+    <col min="36" max="36" width="4" customWidth="true"/>
     <col min="37" max="37" width="7.7109375" customWidth="true"/>
-    <col min="38" max="38" width="13.7109375" customWidth="true"/>
+    <col min="38" max="38" width="15" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>500</v>
+        <v>822</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>504</v>
+        <v>826</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>505</v>
+        <v>827</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>507</v>
+        <v>829</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>508</v>
+        <v>830</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>513</v>
+        <v>835</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>514</v>
+        <v>836</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>515</v>
+        <v>837</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>516</v>
+        <v>838</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>517</v>
+        <v>839</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>518</v>
+        <v>840</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>519</v>
+        <v>841</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>520</v>
+        <v>842</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>521</v>
+        <v>843</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>522</v>
+        <v>844</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>523</v>
+        <v>845</v>
       </c>
       <c r="Q1" s="0" t="s">
-        <v>524</v>
+        <v>846</v>
       </c>
       <c r="R1" s="0" t="s">
-        <v>525</v>
+        <v>847</v>
       </c>
       <c r="S1" s="0" t="s">
-        <v>526</v>
+        <v>848</v>
       </c>
       <c r="T1" s="0" t="s">
-        <v>527</v>
+        <v>849</v>
       </c>
       <c r="U1" s="0" t="s">
-        <v>528</v>
+        <v>850</v>
       </c>
       <c r="V1" s="0" t="s">
-        <v>529</v>
+        <v>851</v>
       </c>
       <c r="W1" s="0" t="s">
-        <v>530</v>
+        <v>852</v>
       </c>
       <c r="X1" s="0" t="s">
-        <v>531</v>
+        <v>853</v>
       </c>
       <c r="Y1" s="0" t="s">
-        <v>532</v>
+        <v>854</v>
       </c>
       <c r="Z1" s="0" t="s">
-        <v>533</v>
+        <v>855</v>
       </c>
       <c r="AA1" s="0" t="s">
-        <v>534</v>
+        <v>856</v>
       </c>
       <c r="AB1" s="0" t="s">
-        <v>535</v>
+        <v>857</v>
       </c>
       <c r="AC1" s="0" t="s">
-        <v>536</v>
+        <v>858</v>
       </c>
       <c r="AD1" s="0" t="s">
-        <v>537</v>
+        <v>859</v>
       </c>
       <c r="AE1" s="0" t="s">
-        <v>538</v>
+        <v>860</v>
       </c>
       <c r="AF1" s="0" t="s">
-        <v>539</v>
+        <v>861</v>
       </c>
       <c r="AG1" s="0" t="s">
-        <v>540</v>
+        <v>862</v>
       </c>
       <c r="AH1" s="0" t="s">
-        <v>541</v>
+        <v>863</v>
       </c>
       <c r="AI1" s="0" t="s">
-        <v>542</v>
+        <v>864</v>
       </c>
       <c r="AJ1" s="0" t="s">
-        <v>543</v>
+        <v>865</v>
       </c>
       <c r="AK1" s="0" t="s">
-        <v>544</v>
+        <v>866</v>
       </c>
       <c r="AL1" s="0" t="s">
-        <v>545</v>
+        <v>867</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>501</v>
+        <v>823</v>
       </c>
       <c r="B2" s="0">
         <v>220519</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>506</v>
+        <v>828</v>
       </c>
       <c r="D2" s="0">
         <v>3</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>509</v>
+        <v>831</v>
       </c>
       <c r="F2" s="0">
         <v>507.31400000000002</v>
@@ -7386,19 +8352,19 @@
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>501</v>
+        <v>823</v>
       </c>
       <c r="B3" s="0">
         <v>290519</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>506</v>
+        <v>828</v>
       </c>
       <c r="D3" s="0">
         <v>1</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>510</v>
+        <v>832</v>
       </c>
       <c r="F3" s="0">
         <v>404.71699999999998</v>
@@ -7500,19 +8466,19 @@
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>502</v>
+        <v>824</v>
       </c>
       <c r="B4" s="0">
         <v>290519</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>506</v>
+        <v>828</v>
       </c>
       <c r="D4" s="0">
         <v>2</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>511</v>
+        <v>833</v>
       </c>
       <c r="F4" s="0">
         <v>585.452</v>
@@ -7614,19 +8580,19 @@
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>503</v>
+        <v>825</v>
       </c>
       <c r="B5" s="0">
         <v>270520</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>506</v>
+        <v>828</v>
       </c>
       <c r="D5" s="0">
         <v>2</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>512</v>
+        <v>834</v>
       </c>
       <c r="F5" s="0">
         <v>393.995</v>
@@ -7931,177 +8897,177 @@
   <dimension ref="A1:AL13"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="5.48828125" customWidth="true"/>
-    <col min="2" max="2" width="7.15625" customWidth="true"/>
-    <col min="3" max="3" width="10.6015625" customWidth="true"/>
-    <col min="4" max="4" width="4.82421875" customWidth="true"/>
-    <col min="5" max="5" width="3.82421875" customWidth="true"/>
+    <col min="1" max="1" width="5.85546875" customWidth="true"/>
+    <col min="2" max="2" width="7.140625" customWidth="true"/>
+    <col min="3" max="3" width="11.5703125" customWidth="true"/>
+    <col min="4" max="4" width="5.28515625" customWidth="true"/>
+    <col min="5" max="5" width="3.85546875" customWidth="true"/>
     <col min="6" max="6" width="7.7109375" customWidth="true"/>
-    <col min="7" max="7" width="10.15625" customWidth="true"/>
-    <col min="8" max="8" width="7.37890625" customWidth="true"/>
-    <col min="9" max="9" width="9.15625" customWidth="true"/>
+    <col min="7" max="7" width="10.85546875" customWidth="true"/>
+    <col min="8" max="8" width="8" customWidth="true"/>
+    <col min="9" max="9" width="10.140625" customWidth="true"/>
     <col min="10" max="10" width="7.7109375" customWidth="true"/>
-    <col min="11" max="11" width="8.7109375" customWidth="true"/>
-    <col min="12" max="12" width="9.26953125" customWidth="true"/>
+    <col min="11" max="11" width="9.42578125" customWidth="true"/>
+    <col min="12" max="12" width="10" customWidth="true"/>
     <col min="13" max="13" width="7.7109375" customWidth="true"/>
     <col min="14" max="14" width="6.7109375" customWidth="true"/>
-    <col min="15" max="15" width="4.37890625" customWidth="true"/>
-    <col min="16" max="16" width="7.93359375" customWidth="true"/>
-    <col min="17" max="17" width="7.82421875" customWidth="true"/>
+    <col min="15" max="15" width="4.7109375" customWidth="true"/>
+    <col min="16" max="16" width="8.140625" customWidth="true"/>
+    <col min="17" max="17" width="8.140625" customWidth="true"/>
     <col min="18" max="18" width="6.7109375" customWidth="true"/>
-    <col min="19" max="19" width="9.37890625" customWidth="true"/>
-    <col min="20" max="20" width="7.37890625" customWidth="true"/>
+    <col min="19" max="19" width="10" customWidth="true"/>
+    <col min="20" max="20" width="8.28515625" customWidth="true"/>
     <col min="21" max="21" width="11.7109375" customWidth="true"/>
-    <col min="22" max="22" width="8.046875" customWidth="true"/>
+    <col min="22" max="22" width="8.85546875" customWidth="true"/>
     <col min="23" max="23" width="11.7109375" customWidth="true"/>
-    <col min="24" max="24" width="10.37890625" customWidth="true"/>
-    <col min="25" max="25" width="11.7109375" customWidth="true"/>
+    <col min="24" max="24" width="10.42578125" customWidth="true"/>
+    <col min="25" max="25" width="12.42578125" customWidth="true"/>
     <col min="26" max="26" width="11.7109375" customWidth="true"/>
     <col min="27" max="27" width="13.7109375" customWidth="true"/>
     <col min="28" max="28" width="12.7109375" customWidth="true"/>
-    <col min="29" max="29" width="10.26953125" customWidth="true"/>
-    <col min="30" max="30" width="11.48828125" customWidth="true"/>
+    <col min="29" max="29" width="11.28515625" customWidth="true"/>
+    <col min="30" max="30" width="13" customWidth="true"/>
     <col min="31" max="31" width="12.7109375" customWidth="true"/>
-    <col min="32" max="32" width="9.15625" customWidth="true"/>
-    <col min="33" max="33" width="7.93359375" customWidth="true"/>
+    <col min="32" max="32" width="10" customWidth="true"/>
+    <col min="33" max="33" width="8.7109375" customWidth="true"/>
     <col min="34" max="34" width="7.7109375" customWidth="true"/>
     <col min="35" max="35" width="11.7109375" customWidth="true"/>
-    <col min="36" max="36" width="3.7109375" customWidth="true"/>
+    <col min="36" max="36" width="4" customWidth="true"/>
     <col min="37" max="37" width="7.7109375" customWidth="true"/>
-    <col min="38" max="38" width="13.7109375" customWidth="true"/>
+    <col min="38" max="38" width="15" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>546</v>
+        <v>868</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>555</v>
+        <v>877</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>556</v>
+        <v>878</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>558</v>
+        <v>880</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>559</v>
+        <v>881</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>572</v>
+        <v>894</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>573</v>
+        <v>895</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>574</v>
+        <v>896</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>575</v>
+        <v>897</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>576</v>
+        <v>898</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>577</v>
+        <v>899</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>578</v>
+        <v>900</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>579</v>
+        <v>901</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>580</v>
+        <v>902</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>581</v>
+        <v>903</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>582</v>
+        <v>904</v>
       </c>
       <c r="Q1" s="0" t="s">
-        <v>583</v>
+        <v>905</v>
       </c>
       <c r="R1" s="0" t="s">
-        <v>584</v>
+        <v>906</v>
       </c>
       <c r="S1" s="0" t="s">
-        <v>585</v>
+        <v>907</v>
       </c>
       <c r="T1" s="0" t="s">
-        <v>586</v>
+        <v>908</v>
       </c>
       <c r="U1" s="0" t="s">
-        <v>587</v>
+        <v>909</v>
       </c>
       <c r="V1" s="0" t="s">
-        <v>588</v>
+        <v>910</v>
       </c>
       <c r="W1" s="0" t="s">
-        <v>589</v>
+        <v>911</v>
       </c>
       <c r="X1" s="0" t="s">
-        <v>590</v>
+        <v>912</v>
       </c>
       <c r="Y1" s="0" t="s">
-        <v>591</v>
+        <v>913</v>
       </c>
       <c r="Z1" s="0" t="s">
-        <v>592</v>
+        <v>914</v>
       </c>
       <c r="AA1" s="0" t="s">
-        <v>593</v>
+        <v>915</v>
       </c>
       <c r="AB1" s="0" t="s">
-        <v>594</v>
+        <v>916</v>
       </c>
       <c r="AC1" s="0" t="s">
-        <v>595</v>
+        <v>917</v>
       </c>
       <c r="AD1" s="0" t="s">
-        <v>596</v>
+        <v>918</v>
       </c>
       <c r="AE1" s="0" t="s">
-        <v>597</v>
+        <v>919</v>
       </c>
       <c r="AF1" s="0" t="s">
-        <v>598</v>
+        <v>920</v>
       </c>
       <c r="AG1" s="0" t="s">
-        <v>599</v>
+        <v>921</v>
       </c>
       <c r="AH1" s="0" t="s">
-        <v>600</v>
+        <v>922</v>
       </c>
       <c r="AI1" s="0" t="s">
-        <v>601</v>
+        <v>923</v>
       </c>
       <c r="AJ1" s="0" t="s">
-        <v>602</v>
+        <v>924</v>
       </c>
       <c r="AK1" s="0" t="s">
-        <v>603</v>
+        <v>925</v>
       </c>
       <c r="AL1" s="0" t="s">
-        <v>604</v>
+        <v>926</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>547</v>
+        <v>869</v>
       </c>
       <c r="B2" s="0">
         <v>31218</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>557</v>
+        <v>879</v>
       </c>
       <c r="D2" s="0">
         <v>2</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>560</v>
+        <v>882</v>
       </c>
       <c r="F2" s="0">
         <v>360.89699999999999</v>
@@ -8201,19 +9167,19 @@
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>547</v>
+        <v>869</v>
       </c>
       <c r="B3" s="0">
         <v>171218</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>557</v>
+        <v>879</v>
       </c>
       <c r="D3" s="0">
         <v>2</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>561</v>
+        <v>883</v>
       </c>
       <c r="F3" s="0">
         <v>457.68700000000001</v>
@@ -8315,19 +9281,19 @@
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>548</v>
+        <v>870</v>
       </c>
       <c r="B4" s="0">
         <v>171218</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>557</v>
+        <v>879</v>
       </c>
       <c r="D4" s="0">
         <v>2</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>562</v>
+        <v>884</v>
       </c>
       <c r="F4" s="0">
         <v>426.435</v>
@@ -8429,19 +9395,19 @@
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>549</v>
+        <v>871</v>
       </c>
       <c r="B5" s="0">
         <v>171218</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>557</v>
+        <v>879</v>
       </c>
       <c r="D5" s="0">
         <v>2</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>563</v>
+        <v>885</v>
       </c>
       <c r="F5" s="0">
         <v>428.84899999999999</v>
@@ -8543,19 +9509,19 @@
     </row>
     <row r="6">
       <c r="A6" s="0" t="s">
-        <v>549</v>
+        <v>871</v>
       </c>
       <c r="B6" s="0">
         <v>171218</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>557</v>
+        <v>879</v>
       </c>
       <c r="D6" s="0">
         <v>3</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>564</v>
+        <v>886</v>
       </c>
       <c r="F6" s="0">
         <v>378.36900000000003</v>
@@ -8657,19 +9623,19 @@
     </row>
     <row r="7">
       <c r="A7" s="0" t="s">
-        <v>550</v>
+        <v>872</v>
       </c>
       <c r="B7" s="0">
         <v>171218</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>557</v>
+        <v>879</v>
       </c>
       <c r="D7" s="0">
         <v>3</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>565</v>
+        <v>887</v>
       </c>
       <c r="F7" s="0">
         <v>416.42399999999998</v>
@@ -8769,19 +9735,19 @@
     </row>
     <row r="8">
       <c r="A8" s="0" t="s">
-        <v>551</v>
+        <v>873</v>
       </c>
       <c r="B8" s="0">
         <v>70219</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>557</v>
+        <v>879</v>
       </c>
       <c r="D8" s="0">
         <v>3</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>566</v>
+        <v>888</v>
       </c>
       <c r="F8" s="0">
         <v>546.37099999999998</v>
@@ -8885,19 +9851,19 @@
     </row>
     <row r="9">
       <c r="A9" s="0" t="s">
-        <v>552</v>
+        <v>874</v>
       </c>
       <c r="B9" s="0">
         <v>80219</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>557</v>
+        <v>879</v>
       </c>
       <c r="D9" s="0">
         <v>2</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>567</v>
+        <v>889</v>
       </c>
       <c r="F9" s="0">
         <v>309.95600000000002</v>
@@ -8999,19 +9965,19 @@
     </row>
     <row r="10">
       <c r="A10" s="0" t="s">
-        <v>553</v>
+        <v>875</v>
       </c>
       <c r="B10" s="0">
         <v>80219</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>557</v>
+        <v>879</v>
       </c>
       <c r="D10" s="0">
         <v>2</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>568</v>
+        <v>890</v>
       </c>
       <c r="F10" s="0">
         <v>500.19600000000003</v>
@@ -9113,19 +10079,19 @@
     </row>
     <row r="11">
       <c r="A11" s="0" t="s">
-        <v>553</v>
+        <v>875</v>
       </c>
       <c r="B11" s="0">
         <v>80219</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>557</v>
+        <v>879</v>
       </c>
       <c r="D11" s="0">
         <v>2</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>569</v>
+        <v>891</v>
       </c>
       <c r="F11" s="0">
         <v>459.149</v>
@@ -9227,19 +10193,19 @@
     </row>
     <row r="12">
       <c r="A12" s="0" t="s">
-        <v>553</v>
+        <v>875</v>
       </c>
       <c r="B12" s="0">
         <v>80219</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>557</v>
+        <v>879</v>
       </c>
       <c r="D12" s="0">
         <v>2</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>570</v>
+        <v>892</v>
       </c>
       <c r="F12" s="0">
         <v>411.88499999999999</v>
@@ -9341,19 +10307,19 @@
     </row>
     <row r="13">
       <c r="A13" s="0" t="s">
-        <v>554</v>
+        <v>876</v>
       </c>
       <c r="B13" s="0">
         <v>150519</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>557</v>
+        <v>879</v>
       </c>
       <c r="D13" s="0">
         <v>2</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>571</v>
+        <v>893</v>
       </c>
       <c r="F13" s="0">
         <v>543.94600000000003</v>

</xml_diff>